<commit_message>
Preparations for downloading the CERNOX sensor calibration from Epics (cont).
</commit_message>
<xml_diff>
--- a/doc/CERNOX/Affectation_CERNOX_GERSEMI.xlsx
+++ b/doc/CERNOX/Affectation_CERNOX_GERSEMI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Freia\freia-drop\08 Equipment\Cryostat02_Gersemi\08 Documentation\Cernox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC76ED1-A840-4B0A-822A-604FE015D865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BE5F6A-2BFE-44B6-86F0-205C74F02BB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>TT679UU</t>
   </si>
   <si>
-    <t>TT686M</t>
-  </si>
-  <si>
     <t>TT662M</t>
   </si>
   <si>
@@ -80,18 +77,6 @@
     <t>TT665M</t>
   </si>
   <si>
-    <t>TT690M</t>
-  </si>
-  <si>
-    <t>TT691M</t>
-  </si>
-  <si>
-    <t>TT692M</t>
-  </si>
-  <si>
-    <t>TT693M</t>
-  </si>
-  <si>
     <t>TT694M</t>
   </si>
   <si>
@@ -140,18 +125,6 @@
     <t>TT671M</t>
   </si>
   <si>
-    <t>TT683M</t>
-  </si>
-  <si>
-    <t>TT684M</t>
-  </si>
-  <si>
-    <t>TT685M</t>
-  </si>
-  <si>
-    <t>TT687M</t>
-  </si>
-  <si>
     <t>TT642CV</t>
   </si>
   <si>
@@ -509,9 +482,6 @@
     <t xml:space="preserve">X121510 </t>
   </si>
   <si>
-    <t>TT688M</t>
-  </si>
-  <si>
     <t>TT694L</t>
   </si>
   <si>
@@ -531,6 +501,36 @@
   </si>
   <si>
     <t>X85706</t>
+  </si>
+  <si>
+    <t>TT683</t>
+  </si>
+  <si>
+    <t>TT684</t>
+  </si>
+  <si>
+    <t>TT685</t>
+  </si>
+  <si>
+    <t>TT686</t>
+  </si>
+  <si>
+    <t>TT687</t>
+  </si>
+  <si>
+    <t>TT688</t>
+  </si>
+  <si>
+    <t>TT690</t>
+  </si>
+  <si>
+    <t>TT691</t>
+  </si>
+  <si>
+    <t>TT692</t>
+  </si>
+  <si>
+    <t>TT693</t>
   </si>
 </sst>
 </file>
@@ -936,82 +936,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1019,15 +1019,15 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1035,279 +1035,279 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1315,15 +1315,15 @@
         <v>2</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1331,31 +1331,31 @@
         <v>3</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1363,15 +1363,15 @@
         <v>4</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1379,15 +1379,15 @@
         <v>5</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1395,7 +1395,7 @@
         <v>6</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>7</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1419,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1427,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>11</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1443,7 +1443,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -1451,193 +1451,193 @@
         <v>13</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>163</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>166</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>167</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B85" s="33" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1661,42 +1661,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>